<commit_message>
Multiply calculation succeeded! Congratulations!
</commit_message>
<xml_diff>
--- a/Draft of emulator.xlsx
+++ b/Draft of emulator.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5724" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5724" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Multiply" sheetId="1" r:id="rId1"/>
     <sheet name="Plus" sheetId="2" r:id="rId2"/>
     <sheet name="Minus" sheetId="3" r:id="rId3"/>
+    <sheet name="Exponentiation" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -536,7 +537,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>X</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -595,6 +596,26 @@
   </si>
   <si>
     <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>num:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>strlen=7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -720,14 +741,14 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1128,11 +1149,11 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D6" s="7">
+      <c r="D6" s="9">
         <f>925841*8</f>
         <v>7406728</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -1518,7 +1539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="V26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="AB35" sqref="AB35:AB36"/>
     </sheetView>
   </sheetViews>
@@ -1576,7 +1597,7 @@
       <c r="D4">
         <v>7</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>7</v>
       </c>
     </row>
@@ -1757,7 +1778,7 @@
       </c>
     </row>
     <row r="36" spans="19:28" x14ac:dyDescent="0.25">
-      <c r="S36" s="8" t="s">
+      <c r="S36" s="7" t="s">
         <v>14</v>
       </c>
       <c r="T36">
@@ -1832,4 +1853,85 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>35.612499999999997</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="14.4" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Multiply calculation succeeded! Congratulations! (Comments available)
</commit_message>
<xml_diff>
--- a/Draft of emulator.xlsx
+++ b/Draft of emulator.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5724" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5724" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Multiply" sheetId="1" r:id="rId1"/>
-    <sheet name="Plus" sheetId="2" r:id="rId2"/>
-    <sheet name="Minus" sheetId="3" r:id="rId3"/>
-    <sheet name="Exponentiation" sheetId="4" r:id="rId4"/>
+    <sheet name="Simple Multiply" sheetId="1" r:id="rId1"/>
+    <sheet name="Normal Multiply" sheetId="5" r:id="rId2"/>
+    <sheet name="Plus" sheetId="2" r:id="rId3"/>
+    <sheet name="Minus" sheetId="3" r:id="rId4"/>
+    <sheet name="Exponentiation" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -623,8 +624,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="177" formatCode="0_ "/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -719,7 +721,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -749,6 +751,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1033,8 +1038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1338,6 +1343,214 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:P4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="16" width="16.77734375" style="10" customWidth="1"/>
+    <col min="17" max="16384" width="8.88671875" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B2" s="10">
+        <f ca="1">RANDBETWEEN(1000,10000000)</f>
+        <v>6678847</v>
+      </c>
+      <c r="C2" s="10">
+        <f t="shared" ref="C2:P3" ca="1" si="0">RANDBETWEEN(1000,10000000)</f>
+        <v>8097172</v>
+      </c>
+      <c r="D2" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>5336037</v>
+      </c>
+      <c r="E2" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>6313277</v>
+      </c>
+      <c r="F2" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>4615812</v>
+      </c>
+      <c r="G2" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>3139809</v>
+      </c>
+      <c r="H2" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>5309712</v>
+      </c>
+      <c r="I2" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>8515028</v>
+      </c>
+      <c r="J2" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>4732092</v>
+      </c>
+      <c r="K2" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>4681212</v>
+      </c>
+      <c r="L2" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>4235210</v>
+      </c>
+      <c r="M2" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>2535125</v>
+      </c>
+      <c r="N2" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>8632722</v>
+      </c>
+      <c r="O2" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>3229784</v>
+      </c>
+      <c r="P2" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>6610962</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B3" s="10">
+        <f ca="1">RANDBETWEEN(1000,10000000)</f>
+        <v>5510435</v>
+      </c>
+      <c r="C3" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>7464940</v>
+      </c>
+      <c r="D3" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>4528514</v>
+      </c>
+      <c r="E3" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>8440045</v>
+      </c>
+      <c r="F3" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>5009613</v>
+      </c>
+      <c r="G3" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>9286740</v>
+      </c>
+      <c r="H3" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>859878</v>
+      </c>
+      <c r="I3" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>1536314</v>
+      </c>
+      <c r="J3" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>4626937</v>
+      </c>
+      <c r="K3" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>4513143</v>
+      </c>
+      <c r="L3" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>2663734</v>
+      </c>
+      <c r="M3" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>2363871</v>
+      </c>
+      <c r="N3" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>7166862</v>
+      </c>
+      <c r="O3" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>6696194</v>
+      </c>
+      <c r="P3" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>3839536</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="10">
+        <f ca="1">B2*B3</f>
+        <v>36803352268445</v>
+      </c>
+      <c r="C4" s="10">
+        <f t="shared" ref="C4:P4" ca="1" si="1">C2*C3</f>
+        <v>60444903149680</v>
+      </c>
+      <c r="D4" s="10">
+        <f t="shared" ca="1" si="1"/>
+        <v>24164318259018</v>
+      </c>
+      <c r="E4" s="10">
+        <f t="shared" ca="1" si="1"/>
+        <v>53284341977465</v>
+      </c>
+      <c r="F4" s="10">
+        <f t="shared" ca="1" si="1"/>
+        <v>23123431800756</v>
+      </c>
+      <c r="G4" s="10">
+        <f t="shared" ca="1" si="1"/>
+        <v>29158589832660</v>
+      </c>
+      <c r="H4" s="10">
+        <f t="shared" ca="1" si="1"/>
+        <v>4565704535136</v>
+      </c>
+      <c r="I4" s="10">
+        <f t="shared" ca="1" si="1"/>
+        <v>13081756726792</v>
+      </c>
+      <c r="J4" s="10">
+        <f t="shared" ca="1" si="1"/>
+        <v>21895091562204</v>
+      </c>
+      <c r="K4" s="10">
+        <f t="shared" ca="1" si="1"/>
+        <v>21126979169316</v>
+      </c>
+      <c r="L4" s="10">
+        <f t="shared" ca="1" si="1"/>
+        <v>11281472874140</v>
+      </c>
+      <c r="M4" s="10">
+        <f t="shared" ca="1" si="1"/>
+        <v>5992708468875</v>
+      </c>
+      <c r="N4" s="10">
+        <f t="shared" ca="1" si="1"/>
+        <v>61869527258364</v>
+      </c>
+      <c r="O4" s="10">
+        <f t="shared" ca="1" si="1"/>
+        <v>21627260242096</v>
+      </c>
+      <c r="P4" s="10">
+        <f t="shared" ca="1" si="1"/>
+        <v>25383026593632</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
@@ -1535,7 +1748,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB37"/>
   <sheetViews>
@@ -1855,11 +2068,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>

</xml_diff>